<commit_message>
refactor(edit-station): add station #
</commit_message>
<xml_diff>
--- a/forms/contact/station-edit.xlsx
+++ b/forms/contact/station-edit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Work/dccms/daily-register/forms/contact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A28FB8-DBCB-F14C-9324-F0AE6DD25818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5AC0C3-37AE-754F-9C45-A755107E943D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>type</t>
   </si>
@@ -197,13 +197,19 @@
   </si>
   <si>
     <t>Edit Station</t>
+  </si>
+  <si>
+    <t>station_number</t>
+  </si>
+  <si>
+    <t>Station number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -215,10 +221,16 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +291,12 @@
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -292,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -321,6 +339,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,13 +723,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF1048575"/>
+  <dimension ref="A1:AF1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1088,7 +1108,7 @@
       <c r="Q9" s="14"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>20</v>
       </c>
@@ -1171,42 +1191,53 @@
       <c r="AF11" s="15"/>
     </row>
     <row r="12" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
+      <c r="AF13" s="15"/>
     </row>
-    <row r="1048550" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048551" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048552" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048553" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1232,6 +1263,7 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1368,7 +1400,7 @@
       </c>
       <c r="C2" s="19" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-04-18 4-29</v>
+        <v>2023-06-27 15-33</v>
       </c>
       <c r="E2" t="s">
         <v>49</v>

</xml_diff>